<commit_message>
add missing translations (in FR)
</commit_message>
<xml_diff>
--- a/tools/nist/nist-csf-2.0.xlsx
+++ b/tools/nist/nist-csf-2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/nist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864A5994-4092-2744-B341-56F183E3E581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD75035-9047-3D4D-9E6E-F9B3F5F1B799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,14 @@
     <sheet name="scores" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">csf!$A$1:$F$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">csf!$A$1:$L$135</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="1012">
   <si>
     <t>assessable</t>
   </si>
@@ -4184,6 +4184,40 @@
   </si>
   <si>
     <t>annotation[es]</t>
+  </si>
+  <si>
+    <t>Le risque de cybersécurité pour l’organisation, les actifs et
+les individus est compris par l’organisation</t>
+  </si>
+  <si>
+    <t>Le personnel de l’organisation reçoit une sensibilisation et une formation à la cybersécurité afin qu’il puisse accomplir ses tâches liées à la cybersécurité</t>
+  </si>
+  <si>
+    <t>Les améliorations aux processus, procédures et activités de gestion des risques de cybersécurité organisationnels sont identifiées dans toutes les Fonctions du CSF.</t>
+  </si>
+  <si>
+    <t>Les données sont gérées conformément à la stratégie de risque de l’organisation afin de protéger la confidentialité, l’intégrité et la disponibilité des informations</t>
+  </si>
+  <si>
+    <t>Le matériel, les logiciels (p. ex., les micrologiciels, les systèmes d’exploitation, les applications) et les services des plateformes physiques et virtuelles sont gérés conformément à la stratégie de risque de l’organisation pour protéger leur confidentialité, leur intégrité et leur disponibilité</t>
+  </si>
+  <si>
+    <t>Les architectures de sécurité sont gérées avec la stratégie de risque de l’organisation pour protéger la confidentialité, l’intégrité et la disponibilité des actifs, ainsi que la résilience organisationnelle</t>
+  </si>
+  <si>
+    <t>Les anomalies, les indicateurs de compromission et d’autres événements potentiellement indésirables sont analysés pour caractériser les événements et détecter les incidents de cybersécurité</t>
+  </si>
+  <si>
+    <t>Des enquêtes sont menées pour garantir une réponse efficace et soutenir les activités criminalistiques et de récupération</t>
+  </si>
+  <si>
+    <t>Les activités de réponse sont coordonnées avec les parties prenantes internes et externes, comme l’exigent les lois, les réglementations ou les politiques</t>
+  </si>
+  <si>
+    <t>Les activités sont réalisées pour empêcher l’expansion d’un événement et atténuer ses effets</t>
+  </si>
+  <si>
+    <t>Les activités de restauration sont coordonnées avec les parties internes et externes</t>
   </si>
 </sst>
 </file>
@@ -4790,19 +4824,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E40" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H136" sqref="H136"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
     <col min="5" max="5" width="71.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="57.6640625" customWidth="1"/>
+    <col min="6" max="6" width="57.6640625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="43.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="238" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="80.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="104.6640625" customWidth="1"/>
+    <col min="9" max="9" width="80.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="33" style="2" customWidth="1"/>
     <col min="11" max="11" width="150.6640625" customWidth="1"/>
     <col min="12" max="12" width="168.6640625" style="2" customWidth="1"/>
@@ -4898,7 +4935,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="80" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4928,7 +4965,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="176" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -4958,7 +4995,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="208" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -4988,7 +5025,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="208" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -5018,7 +5055,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -5074,7 +5111,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="176" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -5104,7 +5141,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="176" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -5134,7 +5171,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="128" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5164,7 +5201,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -5194,7 +5231,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -5224,7 +5261,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="192" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -5254,7 +5291,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="128" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -5310,7 +5347,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="224" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -5340,7 +5377,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="240" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -5370,7 +5407,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -5400,7 +5437,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="208" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -5456,7 +5493,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="272" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="272" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -5486,7 +5523,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="240" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -5542,7 +5579,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -5572,7 +5609,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="128" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -5602,7 +5639,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -5658,7 +5695,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="304" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="304" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -5688,7 +5725,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -5718,7 +5755,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="176" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -5748,7 +5785,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="128" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -5778,7 +5815,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -5808,7 +5845,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="192" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -5838,7 +5875,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="288" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="288" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -5868,7 +5905,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="224" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -5898,7 +5935,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="240" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -5928,7 +5965,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="288" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="288" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -6010,7 +6047,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="80" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -6040,7 +6077,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -6070,7 +6107,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="208" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -6100,7 +6137,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -6130,7 +6167,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -6160,7 +6197,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="192" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -6190,7 +6227,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -6236,6 +6273,9 @@
       <c r="G49" s="2" t="s">
         <v>473</v>
       </c>
+      <c r="H49" s="2" t="s">
+        <v>1001</v>
+      </c>
       <c r="J49" s="2" t="s">
         <v>813</v>
       </c>
@@ -6243,7 +6283,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="256" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="256" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -6273,7 +6313,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -6303,7 +6343,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -6333,7 +6373,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="176" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -6363,7 +6403,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="80" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -6393,7 +6433,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="208" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -6423,7 +6463,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -6453,7 +6493,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -6483,7 +6523,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="64" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -6513,7 +6553,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -6559,6 +6599,9 @@
       <c r="G60" s="2" t="s">
         <v>472</v>
       </c>
+      <c r="H60" s="2" t="s">
+        <v>1003</v>
+      </c>
       <c r="J60" s="2" t="s">
         <v>835</v>
       </c>
@@ -6566,7 +6609,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -6596,7 +6639,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="365" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="365" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -6626,7 +6669,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="112" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -6656,7 +6699,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="320" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="320" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -6738,7 +6781,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="208" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -6768,7 +6811,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" ht="112" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -6798,7 +6841,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -6828,7 +6871,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" ht="192" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -6858,7 +6901,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" ht="224" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -6888,7 +6931,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -6934,6 +6977,9 @@
       <c r="G73" s="2" t="s">
         <v>474</v>
       </c>
+      <c r="H73" s="2" t="s">
+        <v>1002</v>
+      </c>
       <c r="J73" s="2" t="s">
         <v>861</v>
       </c>
@@ -6941,7 +6987,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="256" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="256" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -6971,7 +7017,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="240" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -7017,6 +7063,9 @@
       <c r="G76" s="2" t="s">
         <v>479</v>
       </c>
+      <c r="H76" s="2" t="s">
+        <v>1004</v>
+      </c>
       <c r="J76" s="2" t="s">
         <v>867</v>
       </c>
@@ -7024,7 +7073,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="240" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -7054,7 +7103,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="224" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="224" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -7084,7 +7133,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>11</v>
       </c>
@@ -7114,7 +7163,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -7160,6 +7209,9 @@
       <c r="G81" s="2" t="s">
         <v>478</v>
       </c>
+      <c r="H81" s="2" t="s">
+        <v>1005</v>
+      </c>
       <c r="J81" s="2" t="s">
         <v>877</v>
       </c>
@@ -7167,7 +7219,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -7197,7 +7249,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="272" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" ht="272" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -7227,7 +7279,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -7257,7 +7309,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -7287,7 +7339,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>11</v>
       </c>
@@ -7317,7 +7369,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" ht="128" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -7363,6 +7415,9 @@
       <c r="G88" s="2" t="s">
         <v>475</v>
       </c>
+      <c r="H88" s="2" t="s">
+        <v>1006</v>
+      </c>
       <c r="J88" s="2" t="s">
         <v>891</v>
       </c>
@@ -7370,7 +7425,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="256" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" ht="256" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -7400,7 +7455,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -7430,7 +7485,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="112" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -7460,7 +7515,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" ht="64" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -7542,7 +7597,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" ht="176" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>11</v>
       </c>
@@ -7572,7 +7627,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -7602,7 +7657,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" ht="112" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -7632,7 +7687,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" ht="112" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -7662,7 +7717,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="272" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" ht="272" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -7708,6 +7763,9 @@
       <c r="G100" s="2" t="s">
         <v>477</v>
       </c>
+      <c r="H100" s="2" t="s">
+        <v>1007</v>
+      </c>
       <c r="J100" s="2" t="s">
         <v>915</v>
       </c>
@@ -7715,7 +7773,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" ht="208" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -7745,7 +7803,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" ht="112" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -7775,7 +7833,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" ht="80" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -7805,7 +7863,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" ht="192" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -7835,7 +7893,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" ht="128" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>11</v>
       </c>
@@ -7865,7 +7923,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -7947,7 +8005,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -7977,7 +8035,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" ht="80" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -8007,7 +8065,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -8037,7 +8095,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12" ht="80" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -8067,7 +8125,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -8113,6 +8171,9 @@
       <c r="G114" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="H114" t="s">
+        <v>1008</v>
+      </c>
       <c r="J114" s="2" t="s">
         <v>943</v>
       </c>
@@ -8120,7 +8181,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" ht="176" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -8150,7 +8211,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" ht="144" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -8180,7 +8241,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" ht="80" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -8210,7 +8271,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -8256,6 +8317,9 @@
       <c r="G119" s="2" t="s">
         <v>487</v>
       </c>
+      <c r="H119" t="s">
+        <v>1009</v>
+      </c>
       <c r="J119" s="2" t="s">
         <v>953</v>
       </c>
@@ -8263,7 +8327,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>11</v>
       </c>
@@ -8293,7 +8357,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" ht="240" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -8339,6 +8403,9 @@
       <c r="G122" s="2" t="s">
         <v>488</v>
       </c>
+      <c r="H122" t="s">
+        <v>1010</v>
+      </c>
       <c r="J122" s="2" t="s">
         <v>959</v>
       </c>
@@ -8346,7 +8413,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="208" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" ht="208" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -8376,7 +8443,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="176" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" ht="176" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>11</v>
       </c>
@@ -8458,7 +8525,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -8488,7 +8555,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" ht="80" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>11</v>
       </c>
@@ -8518,7 +8585,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12" ht="64" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -8548,7 +8615,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12" ht="160" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>11</v>
       </c>
@@ -8578,7 +8645,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12" ht="112" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>11</v>
       </c>
@@ -8608,7 +8675,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>11</v>
       </c>
@@ -8654,6 +8721,9 @@
       <c r="G133" s="2" t="s">
         <v>490</v>
       </c>
+      <c r="H133" t="s">
+        <v>1011</v>
+      </c>
       <c r="J133" s="2" t="s">
         <v>981</v>
       </c>
@@ -8661,7 +8731,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="192" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12" ht="192" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>11</v>
       </c>
@@ -8691,7 +8761,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -8722,6 +8792,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L135" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>